<commit_message>
Stanfield start points change
</commit_message>
<xml_diff>
--- a/_static/NoCode/Stanfield Point System.xlsx
+++ b/_static/NoCode/Stanfield Point System.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonathanatwell/My Drive/Home/Teaching/Negotiations/New Cases/NoCode, Inc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CBAF64E-57FD-BC45-9352-C34ED850B908}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A32DFFA-54B8-3341-A12D-6AB55E92BC32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1700" yWindow="6560" windowWidth="28800" windowHeight="17500" xr2:uid="{62CA68C9-CA64-214F-A0B1-9BF6A4C3400C}"/>
+    <workbookView xWindow="2040" yWindow="5940" windowWidth="28800" windowHeight="17500" xr2:uid="{62CA68C9-CA64-214F-A0B1-9BF6A4C3400C}"/>
   </bookViews>
   <sheets>
     <sheet name="Stanfield's Input Sheet" sheetId="1" r:id="rId1"/>
@@ -293,10 +293,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -616,7 +616,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -695,7 +695,7 @@
       <c r="B8" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="20">
+      <c r="C8" s="19">
         <v>0</v>
       </c>
       <c r="D8" s="18">
@@ -749,7 +749,7 @@
     <row r="13" spans="1:4" ht="24" x14ac:dyDescent="0.3">
       <c r="A13" s="11"/>
       <c r="B13" s="11"/>
-      <c r="C13" s="19" t="s">
+      <c r="C13" s="20" t="s">
         <v>27</v>
       </c>
       <c r="D13" s="11"/>
@@ -757,31 +757,31 @@
     <row r="14" spans="1:4" ht="24" x14ac:dyDescent="0.3">
       <c r="A14" s="11"/>
       <c r="B14" s="11"/>
-      <c r="C14" s="19"/>
+      <c r="C14" s="20"/>
       <c r="D14" s="11"/>
     </row>
     <row r="15" spans="1:4" ht="24" x14ac:dyDescent="0.3">
       <c r="A15" s="11"/>
       <c r="B15" s="11"/>
-      <c r="C15" s="19"/>
+      <c r="C15" s="20"/>
       <c r="D15" s="11"/>
     </row>
     <row r="16" spans="1:4" ht="24" x14ac:dyDescent="0.3">
       <c r="A16" s="11"/>
       <c r="B16" s="11"/>
-      <c r="C16" s="19"/>
+      <c r="C16" s="20"/>
       <c r="D16" s="11"/>
     </row>
     <row r="17" spans="1:4" ht="24" x14ac:dyDescent="0.3">
       <c r="A17" s="11"/>
       <c r="B17" s="11"/>
-      <c r="C17" s="19"/>
+      <c r="C17" s="20"/>
       <c r="D17" s="11"/>
     </row>
     <row r="18" spans="1:4" ht="24" x14ac:dyDescent="0.3">
       <c r="A18" s="11"/>
       <c r="B18" s="11"/>
-      <c r="C18" s="19"/>
+      <c r="C18" s="20"/>
       <c r="D18" s="11"/>
     </row>
   </sheetData>
@@ -822,7 +822,7 @@
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1086,7 +1086,7 @@
         <v>21</v>
       </c>
       <c r="B34" s="4">
-        <v>12500</v>
+        <v>9000</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>